<commit_message>
aggiornamento nomi segment cib
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/44_Inst_BusinessLine_CIB.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/44_Inst_BusinessLine_CIB.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michele.dessi\Desktop\WS CIB svil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="26175" windowHeight="11400" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="26175" windowHeight="11400" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Business_Line" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="r Subset_AnalysisUnit" sheetId="10" r:id="rId10"/>
     <sheet name="Fields definition" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="109">
   <si>
     <t>Business_Line</t>
   </si>
@@ -462,9 +462,6 @@
     <t>CREATE/MODIFY</t>
   </si>
   <si>
-    <t>Corporate</t>
-  </si>
-  <si>
     <t>FILTER_CORPORATE</t>
   </si>
   <si>
@@ -483,12 +480,6 @@
     <t>EQUALS</t>
   </si>
   <si>
-    <t>(SEGMENT = 'Corporate')</t>
-  </si>
-  <si>
-    <t>SME_Corporate</t>
-  </si>
-  <si>
     <t>FILTER_SME_CORPORATE</t>
   </si>
   <si>
@@ -519,9 +510,6 @@
     <t>BL_CIB_000003</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
     <t>FI_CIB_0000001</t>
   </si>
   <si>
@@ -594,9 +582,6 @@
     <t>COUNTERPARTY_CIB</t>
   </si>
   <si>
-    <t>(SEGMENT='Small Business')</t>
-  </si>
-  <si>
     <t>COUNTERPARTY_CIB_BL_CIB_00001</t>
   </si>
   <si>
@@ -604,12 +589,24 @@
   </si>
   <si>
     <t>COUNTERPARTY_CIB_BL_CIB_00003</t>
+  </si>
+  <si>
+    <t>(SEGMENT = 'Large Corporate - Corporate')</t>
+  </si>
+  <si>
+    <t>(SEGMENT='Small Business - SME Retail')</t>
+  </si>
+  <si>
+    <t>Large Corporate - Corporate</t>
+  </si>
+  <si>
+    <t>Small Business - SME Retail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1381,6 +1378,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10296525" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11049000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2077,6 +2170,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10639425" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10639425" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2773,6 +2962,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9667875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9667875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3469,6 +3754,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4165,6 +4546,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4861,6 +5338,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9191625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9191625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5557,6 +6130,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10048875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10048875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6253,6 +6922,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6949,6 +7714,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7628,6 +8489,102 @@
           <a:ahLst/>
           <a:cxnLst/>
           <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
@@ -7914,16 +8871,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
@@ -7957,16 +8914,16 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7974,13 +8931,13 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
         <v>106</v>
@@ -7991,16 +8948,16 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -8062,19 +9019,19 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
         <v>102</v>
       </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8082,19 +9039,19 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
         <v>103</v>
       </c>
-      <c r="C4" t="s">
-        <v>108</v>
-      </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8102,19 +9059,19 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
         <v>104</v>
       </c>
-      <c r="C5" t="s">
-        <v>109</v>
-      </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -8128,7 +9085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0"/>
+    <sheetView topLeftCell="A23" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9010,16 +9967,16 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -9030,16 +9987,16 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -9050,16 +10007,16 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -9172,19 +10129,19 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9192,19 +10149,19 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9212,19 +10169,19 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -9286,19 +10243,19 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
         <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9306,19 +10263,19 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9326,19 +10283,19 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -9421,19 +10378,19 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
         <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -9450,19 +10407,19 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J4" t="s">
         <v>45</v>
@@ -9476,19 +10433,19 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
         <v>45</v>
@@ -9508,7 +10465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Aggiunti segment per CIB - Corporate
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/44_Inst_BusinessLine_CIB.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/44_Inst_BusinessLine_CIB.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alberto.collu\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="26175" windowHeight="11400" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="26175" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Business_Line" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="135">
   <si>
     <t>Business_Line</t>
   </si>
@@ -601,13 +601,91 @@
   </si>
   <si>
     <t>Small Business - SME Retail</t>
+  </si>
+  <si>
+    <t>BL_CIB_000004</t>
+  </si>
+  <si>
+    <t>BL_CIB_000005</t>
+  </si>
+  <si>
+    <t>Speculative real estate finance</t>
+  </si>
+  <si>
+    <t>(SEGMENT = 'Speculative real estate finance')</t>
+  </si>
+  <si>
+    <t>Specialized Lending</t>
+  </si>
+  <si>
+    <t>(SEGMENT = 'Specialized Lending')</t>
+  </si>
+  <si>
+    <t>FI_CIB_0000004</t>
+  </si>
+  <si>
+    <t>FI_CIB_0000005</t>
+  </si>
+  <si>
+    <t>FILTER_Speculative_real_estate_finance</t>
+  </si>
+  <si>
+    <t>FILTER_Specialized_Lending</t>
+  </si>
+  <si>
+    <t>R_FILTER_CIB_VAR_04</t>
+  </si>
+  <si>
+    <t>R_FILTER_CIB_VAR_05</t>
+  </si>
+  <si>
+    <t>Speculative_real_estate_finance</t>
+  </si>
+  <si>
+    <t>Specialized_Lending</t>
+  </si>
+  <si>
+    <t>R_FILTER_CIB_OPERATOR_04</t>
+  </si>
+  <si>
+    <t>R_FILTER_CIB_OPERATOR_05</t>
+  </si>
+  <si>
+    <t>Speculative_real_estate_finance_EQUALS</t>
+  </si>
+  <si>
+    <t>Specialized_Lending_EQUALS</t>
+  </si>
+  <si>
+    <t>FV_CIB_0000004</t>
+  </si>
+  <si>
+    <t>FV_CIB_0000005</t>
+  </si>
+  <si>
+    <t>FILTER_CIB_VAR_Speculative_real_estate_finance</t>
+  </si>
+  <si>
+    <t>FILTER_CIB_VAR_Specialized_Lending</t>
+  </si>
+  <si>
+    <t>BRAU_CIB_0000004</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_CIB_BL_CIB_00004</t>
+  </si>
+  <si>
+    <t>BRAU_CIB_0000005</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_CIB_BL_CIB_00005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -632,6 +710,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -660,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -668,6 +752,9 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +789,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -745,7 +838,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -793,7 +892,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -841,7 +946,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -889,7 +1000,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -937,7 +1054,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -985,7 +1108,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1033,7 +1162,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1081,7 +1216,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1129,7 +1270,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1177,7 +1324,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1233,7 +1386,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1289,7 +1448,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1345,7 +1510,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1393,7 +1564,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1441,7 +1618,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1450,6 +1633,114 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="11049000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11220450" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEC26290-3CBA-41ED-AB57-A8749546C154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11401425" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1494,7 +1785,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10242" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="10242" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002280000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1537,7 +1834,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1585,7 +1888,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1633,7 +1942,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1681,7 +1996,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1729,7 +2050,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1777,7 +2104,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1825,7 +2158,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1873,7 +2212,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1921,7 +2266,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1969,7 +2320,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2025,7 +2382,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2081,7 +2444,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2137,7 +2506,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2185,7 +2560,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2233,7 +2614,121 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10639425" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10639425" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C98B35F8-48E5-409A-A747-B02D9865E262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2286,7 +2781,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2329,7 +2830,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2377,7 +2884,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2425,7 +2938,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2473,7 +2992,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2521,7 +3046,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2569,7 +3100,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2617,7 +3154,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2665,7 +3208,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2713,7 +3262,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2761,7 +3316,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2817,7 +3378,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2873,7 +3440,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2929,7 +3502,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2977,7 +3556,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3025,7 +3610,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3034,6 +3625,114 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="9667875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9667875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{803BD132-F2FB-4C3A-A673-205E27B363DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10639425" cy="9534525"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3078,7 +3777,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3074" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="3074" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000020C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3121,7 +3826,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3169,7 +3880,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3217,7 +3934,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3265,7 +3988,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3313,7 +4042,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3361,7 +4096,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3409,7 +4150,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3457,7 +4204,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3505,7 +4258,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3553,7 +4312,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3609,7 +4374,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3665,7 +4436,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3721,7 +4498,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3769,7 +4552,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3817,7 +4606,121 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61523057-F5C2-4627-A99F-1A714184A84B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3870,7 +4773,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4098" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="4098" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002100000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3913,7 +4822,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3961,7 +4876,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4009,7 +4930,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4057,7 +4984,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4105,7 +5038,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4153,7 +5092,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4201,7 +5146,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4249,7 +5200,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4297,7 +5254,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4345,7 +5308,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4401,7 +5370,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4457,7 +5432,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4513,7 +5494,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4561,7 +5548,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4609,7 +5602,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4618,6 +5617,114 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10058400" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E0A292-58D6-4150-BC85-9926FA9761E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10582275" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4662,7 +5769,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5122" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="5122" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002140000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4705,7 +5818,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4753,7 +5872,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4801,7 +5926,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4849,7 +5980,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4897,7 +6034,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4945,7 +6088,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4993,7 +6142,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5041,7 +6196,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5089,7 +6250,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5137,7 +6304,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5193,7 +6366,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5249,7 +6428,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5305,7 +6490,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5353,7 +6544,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5401,7 +6598,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5410,6 +6613,114 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="9191625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9191625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1606F823-9F68-4EB4-A86A-0274032B6D1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11401425" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5454,7 +6765,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6146" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="6146" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002180000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5497,7 +6814,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5545,7 +6868,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5593,7 +6922,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5641,7 +6976,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5689,7 +7030,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5737,7 +7084,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5785,7 +7138,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5833,7 +7192,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5881,7 +7246,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5929,7 +7300,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5985,7 +7362,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6041,7 +7424,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6097,7 +7486,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6145,7 +7540,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6193,7 +7594,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6202,6 +7609,114 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10048875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10048875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D74E9B2B-6C14-4F34-A0DA-CFC8D81D540C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11363325" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6246,7 +7761,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7170" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="7170" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-0000021C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6289,7 +7810,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6337,7 +7864,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6385,7 +7918,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6433,7 +7972,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6481,7 +8026,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6529,7 +8080,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6577,7 +8134,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6625,7 +8188,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6673,7 +8242,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6721,7 +8296,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6777,7 +8358,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6833,7 +8420,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6889,7 +8482,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6937,7 +8536,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6985,7 +8590,121 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6457C45D-E771-4499-8296-EDE43A0DF387}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7038,7 +8757,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8194" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="8194" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002200000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7081,7 +8806,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7129,7 +8860,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7177,7 +8914,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7225,7 +8968,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7273,7 +9022,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7321,7 +9076,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7369,7 +9130,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7417,7 +9184,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7465,7 +9238,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7513,7 +9292,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7569,7 +9354,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7625,7 +9416,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7681,7 +9478,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7729,7 +9532,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7777,7 +9586,121 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A05F3E4C-E91F-46EE-B97B-2AE19596135D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7830,7 +9753,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9218" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="9218" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002240000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7873,7 +9802,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7921,7 +9856,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7969,7 +9910,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8017,7 +9964,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8065,7 +10018,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8113,7 +10072,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8161,7 +10126,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8209,7 +10180,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8257,7 +10234,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8305,7 +10288,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8361,7 +10350,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8417,7 +10412,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8473,7 +10474,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8521,7 +10528,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8569,7 +10582,121 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C2F4F87-2C6C-4519-92E8-72D69BC8EF94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8868,19 +10995,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
@@ -8960,19 +11087,54 @@
         <v>74</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9071,6 +11233,46 @@
         <v>77</v>
       </c>
       <c r="F5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
         <v>101</v>
       </c>
     </row>
@@ -9916,17 +12118,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
@@ -10019,6 +12221,46 @@
         <v>77</v>
       </c>
       <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -10079,17 +12321,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="6" width="19.42578125" customWidth="1"/>
   </cols>
@@ -10181,6 +12423,46 @@
         <v>80</v>
       </c>
       <c r="F5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" t="s">
         <v>86</v>
       </c>
     </row>
@@ -10193,18 +12475,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10295,6 +12576,46 @@
         <v>80</v>
       </c>
       <c r="F5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" t="s">
         <v>67</v>
       </c>
     </row>
@@ -10307,17 +12628,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="17.42578125" customWidth="1"/>
@@ -10454,6 +12775,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10465,7 +12826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>